<commit_message>
updated 2 scrum questions 8 faite
</commit_message>
<xml_diff>
--- a/prepa_certif_updated_scrum_questions_8_faite.xlsx
+++ b/prepa_certif_updated_scrum_questions_8_faite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Salon\m\SAVE_LOCALE\0_FORMATIONS\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00FBD94-7BFB-473F-B0BC-BDEC2B59ED10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99272259-C46F-41F7-9F34-C7C9AEFFD9E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="888" windowWidth="14868" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7272" yWindow="984" windowWidth="14868" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Burndown chart</t>
   </si>
@@ -235,101 +235,6 @@
 déviation</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancellation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : PO only (OR </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>if sprint goal obsolete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">).
-La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
-Le sprint est le SEUL moment dans lequel </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>on n'inspecte pas et on n'adapte pas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dev team, 15 minutes peu importe la taille de l'équipe, le scrum master ne la "conduit" pas.
-PAS DE FORMAT DEFINI : </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>questions ou discussion, tout est possible.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider la dev team, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
-    </r>
-  </si>
-  <si>
     <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU "a revisited product backlog". 
 C'est pour les key stakeholders, scrum master, dev team, PO.    It's not JUST a demo.</t>
   </si>
@@ -365,172 +270,6 @@
   <si>
     <t>Le PO, dev team. "consume not more than 10%", not for the current sprint in progress.
 Ongoing process, act of adding detail, no more than 10% of the capacity of the dev team.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">sprint backlog, product backlog, increment.   
-Inspect frequently, but it should not get in the way of the work.   
-PILARS : Transparency (responsable scrum master), adaptation, inspection. Le PO monitore.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Increment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : somme de tous les product backlog items and the value, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fait par la dev team,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> géré par le PO, sprint goal provides guidance.
-Si retard dû à un </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>élément manquant</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, être sûr d'avoir des tâches à faire pour le prochain sprint en attendant.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Interêts : le produit, la valeur, les key stakholder ( le PO prend le feedback de ces derniers).
-monitoring progress toward high-level </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>goals.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   He is the chief product </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>visionary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>KVA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : current value, ability to innovate, time-to-market (expert).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pas le problème du PO :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> coach the dev team, remove impediments to the dev team.
-Iterating vision every sprint, planning features, articulating the product vision (early and often).
-Releases ? the risk for the value, absorption by the customer, the costs and benefits, the constraints by the new release.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -626,97 +365,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
-Sert à </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>améliorer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour les prochains sprints, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>analyser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
-if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>improvement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Responsable: PO uniquement.
 La dev team peut faire des changements </t>
     </r>
@@ -1087,6 +735,362 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sa responsabilité : la product backlog, pas le produit ni du delivery.
+Interêts : le produit, la valeur, les key stakholder ( le PO prend le feedback de ces derniers).
+monitoring progress toward high-level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>goals.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   He is the chief product </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KVA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : current value, ability to innovate, time-to-market (expert).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pas le problème du PO :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> coach the dev team, remove impediments to the dev team.
+Iterating vision every sprint, planning features, articulating the product vision (early and often).
+Releases ? the risk for the value, absorption by the customer, the costs and benefits, the constraints by the new release.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dev team, 15 minutes peu importe la taille de l'équipe, tous les jours, le matin ou l'après-midi.
+PAS DE FORMAT DEFINI : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>questions ou discussion, tout est possible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, le scrum master ne la "conduit" pas.
+3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider la dev team, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancellation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : PO only (OR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if sprint goal obsolete ( ou inatteignable)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
+Le sprint est le SEUL moment dans lequel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on n'inspecte pas et on n'adapte pas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sprint backlog, product backlog, defintion of done, increment (à voir).   
+Inspect frequently, but it should not get in the way of the work.   
+PILARS : Transparency (responsable scrum master), adaptation, inspection. Le PO monitore.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Increment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : somme de tous les product backlog items and the value, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fait par la dev team,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> géré par le PO, sprint goal provides guidance.
+Si retard dû à un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>élément manquant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, être sûr d'avoir des tâches à faire pour le prochain sprint en attendant.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
+( pour les processus) Sert à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>améliorer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour les prochains sprints, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>analyser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
+if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>improvement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
+    </r>
+  </si>
+  <si>
+    <t>user-story, velocity, definition of ready, agile &gt;&gt; tous ces termes n'existent pas dans le guide scrum.</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1510,7 +1514,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1519,7 +1523,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1528,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1537,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1546,16 +1550,16 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:2" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1564,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1600,7 +1604,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1609,16 +1613,16 @@
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1627,7 +1631,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1636,10 +1640,15 @@
         <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>